<commit_message>
Backup QR Scanner data - 2026-01-17T12:27:09.031Z - Cache Bust: 1768652829031
</commit_message>
<xml_diff>
--- a/log_history/Y5_B2526_Neurology_scanner1768638895019_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
+++ b/log_history/Y5_B2526_Neurology_scanner1768638895019_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Session" sheetId="1" r:id="rId1"/>
+    <sheet name="Neurology" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -982,9 +982,69 @@
         <v>emp17.farah.a.youssef@gmail.com</v>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>212572</v>
+      </c>
+      <c r="B30" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C30" t="str">
+        <v>17/01/2026</v>
+      </c>
+      <c r="D30" t="str">
+        <v>14:26:55</v>
+      </c>
+      <c r="E30" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F30" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>213007</v>
+      </c>
+      <c r="B31" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C31" t="str">
+        <v>17/01/2026</v>
+      </c>
+      <c r="D31" t="str">
+        <v>14:26:59</v>
+      </c>
+      <c r="E31" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F31" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>213006</v>
+      </c>
+      <c r="B32" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C32" t="str">
+        <v>17/01/2026</v>
+      </c>
+      <c r="D32" t="str">
+        <v>14:27:03</v>
+      </c>
+      <c r="E32" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F32" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F29"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F32"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update edited session - 2026-01-17T20:30:14.845Z - Cache Bust ID: 176868181484509sktpmv4
</commit_message>
<xml_diff>
--- a/log_history/Y5_B2526_Neurology_scanner1768638895019_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
+++ b/log_history/Y5_B2526_Neurology_scanner1768638895019_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Neurology" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -982,69 +982,9 @@
         <v>emp17.farah.a.youssef@gmail.com</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" t="str">
-        <v>212572</v>
-      </c>
-      <c r="B30" t="str">
-        <v>Neurology</v>
-      </c>
-      <c r="C30" t="str">
-        <v>17/01/2026</v>
-      </c>
-      <c r="D30" t="str">
-        <v>14:26:55</v>
-      </c>
-      <c r="E30" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F30" t="str">
-        <v>emp17.farah.a.youssef@gmail.com</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="str">
-        <v>213007</v>
-      </c>
-      <c r="B31" t="str">
-        <v>Neurology</v>
-      </c>
-      <c r="C31" t="str">
-        <v>17/01/2026</v>
-      </c>
-      <c r="D31" t="str">
-        <v>14:26:59</v>
-      </c>
-      <c r="E31" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F31" t="str">
-        <v>emp17.farah.a.youssef@gmail.com</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="str">
-        <v>213006</v>
-      </c>
-      <c r="B32" t="str">
-        <v>Neurology</v>
-      </c>
-      <c r="C32" t="str">
-        <v>17/01/2026</v>
-      </c>
-      <c r="D32" t="str">
-        <v>14:27:03</v>
-      </c>
-      <c r="E32" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F32" t="str">
-        <v>emp17.farah.a.youssef@gmail.com</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F32"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F29"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>